<commit_message>
Baseline without standard specific schemas.
</commit_message>
<xml_diff>
--- a/import-files/cdash-1-1.xlsx
+++ b/import-files/cdash-1-1.xlsx
@@ -26,7 +26,7 @@
     <definedName name="sdtmig_3_1_2_export_02_dataset" localSheetId="3">'cdash-1-1-dom'!$A$1:$G$34</definedName>
     <definedName name="sdtmig_3_1_2_export_03_data_element_1" localSheetId="4">'cdash-1-1-de'!$A$1:$H$671</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6209" uniqueCount="2919">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6209" uniqueCount="2920">
   <si>
     <t>mms:context</t>
   </si>
@@ -8846,6 +8846,9 @@
   </si>
   <si>
     <t>Recommended/Conditional (R/C): A data collection field that should be on a CRF based on certain conditions (e.g., complete date of birth is preferred, but may not be allowed in some regions; AE time should only be captured if there is another data point with which to compare it). In the absence of this data point other data points would be less meaningful.</t>
+  </si>
+  <si>
+    <t>skos:definition</t>
   </si>
 </sst>
 </file>
@@ -10492,7 +10495,7 @@
         <v>2913</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>33</v>
+        <v>2919</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.25">

</xml_diff>